<commit_message>
Fixed bug in probability calculator that wouldn't assign appropriate probabilities on certain edge cases
</commit_message>
<xml_diff>
--- a/transition_probability_monster.xlsx
+++ b/transition_probability_monster.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaheg\Desktop\ECE 209AS\gridworld\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEF0434-391A-4913-B58C-221D61E34C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04325E1-4EC2-47EA-ABF9-0F20DF4FC68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,7 +401,7 @@
   <dimension ref="A1:A3126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A3126" sqref="A1:A3126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +543,7 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
@@ -1843,7 +1843,7 @@
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
@@ -1973,7 +1973,7 @@
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
@@ -3013,7 +3013,7 @@
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A522">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
@@ -3143,7 +3143,7 @@
     </row>
     <row r="548" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A548">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="549" spans="1:1" x14ac:dyDescent="0.25">
@@ -3273,7 +3273,7 @@
     </row>
     <row r="574" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A574">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="575" spans="1:1" x14ac:dyDescent="0.25">
@@ -3403,7 +3403,7 @@
     </row>
     <row r="600" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A600">
-        <v>0.05</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="601" spans="1:1" x14ac:dyDescent="0.25">
@@ -3533,7 +3533,7 @@
     </row>
     <row r="626" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A626">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="627" spans="1:1" x14ac:dyDescent="0.25">
@@ -4058,7 +4058,7 @@
     </row>
     <row r="731" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A731">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="732" spans="1:1" x14ac:dyDescent="0.25">
@@ -4188,7 +4188,7 @@
     </row>
     <row r="757" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A757">
-        <v>0.1</v>
+        <v>0.97500000000000009</v>
       </c>
     </row>
     <row r="758" spans="1:1" x14ac:dyDescent="0.25">
@@ -4318,7 +4318,7 @@
     </row>
     <row r="783" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A783">
-        <v>0.05</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="784" spans="1:1" x14ac:dyDescent="0.25">
@@ -4708,7 +4708,7 @@
     </row>
     <row r="861" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A861">
-        <v>0.05</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="862" spans="1:1" x14ac:dyDescent="0.25">
@@ -5358,7 +5358,7 @@
     </row>
     <row r="991" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A991">
-        <v>0.05</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="992" spans="1:1" x14ac:dyDescent="0.25">
@@ -5488,7 +5488,7 @@
     </row>
     <row r="1017" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1017">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="1018" spans="1:1" x14ac:dyDescent="0.25">
@@ -5618,7 +5618,7 @@
     </row>
     <row r="1043" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1043">
-        <v>0.05</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="1044" spans="1:1" x14ac:dyDescent="0.25">
@@ -6008,7 +6008,7 @@
     </row>
     <row r="1121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1121">
-        <v>0.05</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="1122" spans="1:1" x14ac:dyDescent="0.25">
@@ -6658,12 +6658,12 @@
     </row>
     <row r="1251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1251">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="1252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1252">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="1253" spans="1:1" x14ac:dyDescent="0.25">
@@ -6793,7 +6793,7 @@
     </row>
     <row r="1278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1278">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="1279" spans="1:1" x14ac:dyDescent="0.25">
@@ -6923,7 +6923,7 @@
     </row>
     <row r="1304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1304">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="1305" spans="1:1" x14ac:dyDescent="0.25">
@@ -7053,7 +7053,7 @@
     </row>
     <row r="1330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1330">
-        <v>0.05</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="1331" spans="1:1" x14ac:dyDescent="0.25">
@@ -7183,7 +7183,7 @@
     </row>
     <row r="1356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1356">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="1357" spans="1:1" x14ac:dyDescent="0.25">
@@ -7313,7 +7313,7 @@
     </row>
     <row r="1382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1382">
-        <v>0.1</v>
+        <v>0.97500000000000009</v>
       </c>
     </row>
     <row r="1383" spans="1:1" x14ac:dyDescent="0.25">
@@ -8093,7 +8093,7 @@
     </row>
     <row r="1538" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1538">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="1539" spans="1:1" x14ac:dyDescent="0.25">
@@ -8223,7 +8223,7 @@
     </row>
     <row r="1564" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1564">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="1565" spans="1:1" x14ac:dyDescent="0.25">
@@ -9393,7 +9393,7 @@
     </row>
     <row r="1798" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1798">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="1799" spans="1:1" x14ac:dyDescent="0.25">
@@ -9523,7 +9523,7 @@
     </row>
     <row r="1824" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1824">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="1825" spans="1:1" x14ac:dyDescent="0.25">
@@ -9788,7 +9788,7 @@
     </row>
     <row r="1877" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1877">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="1878" spans="1:1" x14ac:dyDescent="0.25">
@@ -10438,7 +10438,7 @@
     </row>
     <row r="2007" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2007">
-        <v>0.1</v>
+        <v>0.97500000000000009</v>
       </c>
     </row>
     <row r="2008" spans="1:1" x14ac:dyDescent="0.25">
@@ -10698,7 +10698,7 @@
     </row>
     <row r="2059" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2059">
-        <v>0.05</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="2060" spans="1:1" x14ac:dyDescent="0.25">
@@ -10828,7 +10828,7 @@
     </row>
     <row r="2085" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2085">
-        <v>0.05</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="2086" spans="1:1" x14ac:dyDescent="0.25">
@@ -11088,7 +11088,7 @@
     </row>
     <row r="2137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2137">
-        <v>0.05</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="2138" spans="1:1" x14ac:dyDescent="0.25">
@@ -11738,7 +11738,7 @@
     </row>
     <row r="2267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2267">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="2268" spans="1:1" x14ac:dyDescent="0.25">
@@ -11998,7 +11998,7 @@
     </row>
     <row r="2319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2319">
-        <v>0.05</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="2320" spans="1:1" x14ac:dyDescent="0.25">
@@ -12128,7 +12128,7 @@
     </row>
     <row r="2345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2345">
-        <v>0.05</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="2346" spans="1:1" x14ac:dyDescent="0.25">
@@ -12388,7 +12388,7 @@
     </row>
     <row r="2397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2397">
-        <v>7.5000000000000011E-2</v>
+        <v>0.95000000000000007</v>
       </c>
     </row>
     <row r="2398" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>